<commit_message>
updated compat schema with latest
</commit_message>
<xml_diff>
--- a/compat/tablesSchema.2.0.0.xlsx
+++ b/compat/tablesSchema.2.0.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_workspace\tse_workspace\tse-data-reporting-tool\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_workspace\tse_workspace\tse-reporting-tool\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DA328D-C958-4D55-9670-3723066BEDD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59261BAE-F68C-49E1-ABD1-3881F2019FBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="690" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="690" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="475">
   <si>
     <t>Type</t>
   </si>
@@ -1095,9 +1095,6 @@
     <t>SCRAPIE$AT12A</t>
   </si>
   <si>
-    <t>CWD$AT12A</t>
-  </si>
-  <si>
     <t>RELATION{SummarizedInformation,progId.label}|.|ZERO_PADDING({rowId},6)</t>
   </si>
   <si>
@@ -1167,15 +1164,9 @@
     <t>progIdSuffix</t>
   </si>
   <si>
-    <t>AND((%anMethType.code==AT13A),(RELATION{SummarizedInformation,source.code}==F01.A057G))</t>
-  </si>
-  <si>
     <t>IF(OR((%internalOpType.label==Reject),(%internalOpType.label==Submit)),No,Yes)</t>
   </si>
   <si>
-    <t>(RELATION{SummarizedInformation,source.code}==F01.A057G)</t>
-  </si>
-  <si>
     <t>RELATION{SummarizedInformation,source.code}</t>
   </si>
   <si>
@@ -1320,9 +1311,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>IF(OR((%country.code==EE),(%country.code==FI),(%country.code==LV),(%country.code==LT),(%country.code==PL),(%country.code==SE)),Y,ALL)</t>
-  </si>
-  <si>
     <t>OR((%type.code==CWD),(%type.code==BSEOS))</t>
   </si>
   <si>
@@ -1449,9 +1437,6 @@
     <t>IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),F,)</t>
   </si>
   <si>
-    <t>2010 to 2020</t>
-  </si>
-  <si>
     <t>POS</t>
   </si>
   <si>
@@ -1459,6 +1444,18 @@
   </si>
   <si>
     <t>%country.code|RIGHT_TRIM(%reportYear.code,2)|RIGHT_TRIM(ZERO_PADDING(%reportMonth.code,2),2)</t>
+  </si>
+  <si>
+    <t>CWD$AT11A</t>
+  </si>
+  <si>
+    <t>2021 to 2050</t>
+  </si>
+  <si>
+    <t>OR((RELATION{SummarizedInformation,source.code}==F01.A057G),(RELATION{SummarizedInformation,source.code}==F01.A057P))</t>
+  </si>
+  <si>
+    <t>IF((%anMethType.code==AT13A),OR((RELATION{SummarizedInformation,source.code}==F01.A057G),(RELATION{SummarizedInformation,source.code}==F01.A057P)),No)</t>
   </si>
 </sst>
 </file>
@@ -1594,7 +1591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1620,7 +1617,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1629,6 +1625,8 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3835,7 +3833,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
@@ -3955,16 +3953,16 @@
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="F3" s="24" t="s">
         <v>12</v>
@@ -3982,16 +3980,16 @@
         <v>9</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>421</v>
-      </c>
-      <c r="L3" s="25" t="s">
-        <v>429</v>
+        <v>418</v>
+      </c>
+      <c r="L3" s="31" t="s">
+        <v>419</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>9</v>
@@ -4073,7 +4071,7 @@
         <v>112</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="R5" s="2">
         <v>4</v>
@@ -4245,25 +4243,25 @@
       <c r="E10" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="25" t="s">
         <v>93</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="26" t="s">
+      <c r="I10" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="L10" s="27" t="s">
+      <c r="L10" s="26" t="s">
         <v>352</v>
       </c>
       <c r="R10" s="2">
@@ -4284,25 +4282,25 @@
       <c r="E11" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="25" t="s">
         <v>93</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="K11" s="26" t="s">
+      <c r="I11" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="L11" s="27" t="s">
+      <c r="L11" s="26" t="s">
         <v>353</v>
       </c>
       <c r="R11" s="2">
@@ -4323,26 +4321,26 @@
       <c r="E12" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="27" t="s">
         <v>93</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12" s="28" t="s">
+      <c r="I12" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="L12" s="27" t="s">
-        <v>354</v>
+      <c r="L12" s="26" t="s">
+        <v>471</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
@@ -4367,10 +4365,10 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4470,7 +4468,7 @@
       <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>472</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -4483,7 +4481,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="8" t="s">
@@ -4585,10 +4583,10 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4714,7 +4712,7 @@
       <c r="C8" s="17"/>
       <c r="D8" s="18"/>
       <c r="E8" s="17" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>174</v>
@@ -4745,13 +4743,13 @@
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="18"/>
       <c r="E9" s="17" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>174</v>
@@ -4782,13 +4780,13 @@
     </row>
     <row r="10" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
       <c r="E10" s="17" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>174</v>
@@ -4826,10 +4824,10 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>174</v>
@@ -4869,10 +4867,10 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>174</v>
@@ -4905,15 +4903,15 @@
     </row>
     <row r="13" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>370</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>371</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="18"/>
       <c r="E13" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>174</v>
@@ -4955,8 +4953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="P23" sqref="P23"/>
@@ -5108,7 +5106,7 @@
         <v>3</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>3</v>
@@ -5120,10 +5118,10 @@
         <v>311</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
@@ -5143,7 +5141,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>69</v>
@@ -5158,7 +5156,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>3</v>
@@ -5202,10 +5200,10 @@
         <v>74</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>3</v>
@@ -5246,10 +5244,10 @@
         <v>18</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>3</v>
@@ -5272,40 +5270,40 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="L7" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="L7" s="28" t="s">
         <v>311</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="6" t="s">
@@ -5329,10 +5327,10 @@
         <v>89</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>12</v>
@@ -5341,10 +5339,10 @@
         <v>90</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>3</v>
@@ -5352,14 +5350,14 @@
       <c r="K8" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="L8" s="29" t="s">
-        <v>463</v>
+      <c r="L8" s="28" t="s">
+        <v>459</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>9</v>
@@ -5382,10 +5380,10 @@
         <v>92</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>12</v>
@@ -5394,10 +5392,10 @@
         <v>93</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>3</v>
@@ -5406,13 +5404,13 @@
         <v>112</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="Q9" s="6" t="s">
         <v>9</v>
@@ -5432,7 +5430,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>36</v>
@@ -5444,10 +5442,10 @@
         <v>37</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>3</v>
@@ -5459,10 +5457,10 @@
         <v>311</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="Q10" s="6" t="s">
         <v>5</v>
@@ -5476,23 +5474,23 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>202</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>174</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="6" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>3</v>
@@ -5518,7 +5516,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>238</v>
@@ -5527,16 +5525,16 @@
         <v>8</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -5565,16 +5563,16 @@
         <v>8</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>5</v>
@@ -5603,16 +5601,16 @@
         <v>8</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>5</v>
@@ -5632,7 +5630,7 @@
         <v>20</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>238</v>
@@ -5641,19 +5639,19 @@
         <v>8</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
@@ -5682,16 +5680,16 @@
         <v>8</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>5</v>
@@ -5711,7 +5709,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>174</v>
@@ -5729,7 +5727,7 @@
         <v>3</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>9</v>
@@ -5756,10 +5754,10 @@
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="6" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>3</v>
@@ -5768,7 +5766,7 @@
         <v>318</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>5</v>
@@ -5798,10 +5796,10 @@
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="6" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>3</v>
@@ -5810,7 +5808,7 @@
         <v>318</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>5</v>
@@ -5938,7 +5936,7 @@
         <v>4</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>9</v>
@@ -6025,7 +6023,7 @@
         <v>4</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="Q26" s="6" t="s">
         <v>9</v>
@@ -6054,7 +6052,7 @@
         <v>4</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="Q27" s="6" t="s">
         <v>3</v>
@@ -6176,7 +6174,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -6208,7 +6206,7 @@
         <v>4</v>
       </c>
       <c r="P32" s="6" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>9</v>
@@ -6272,7 +6270,7 @@
         <v>4</v>
       </c>
       <c r="P34" s="6" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="Q34" s="6" t="s">
         <v>9</v>
@@ -6304,7 +6302,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>9</v>
@@ -6312,13 +6310,13 @@
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>174</v>
@@ -6333,7 +6331,7 @@
         <v>4</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="Q36" s="6" t="s">
         <v>9</v>
@@ -6400,7 +6398,7 @@
         <v>4</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>9</v>
@@ -6461,7 +6459,7 @@
         <v>4</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="Q40" s="6" t="s">
         <v>9</v>
@@ -6536,10 +6534,10 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6626,13 +6624,13 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B2" t="s">
         <v>191</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>211</v>
@@ -6644,10 +6642,10 @@
         <v>319</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>3</v>
@@ -6735,10 +6733,10 @@
         <v>302</v>
       </c>
       <c r="M4" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>366</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>367</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>5</v>
@@ -6752,40 +6750,40 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>459</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>449</v>
+        <v>455</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>445</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -6814,10 +6812,10 @@
         <v>74</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>4</v>
@@ -6826,7 +6824,7 @@
         <v>111</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>5</v>
@@ -6855,7 +6853,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>3</v>
@@ -6893,7 +6891,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>3</v>
@@ -7037,7 +7035,7 @@
         <v>217</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>3</v>
@@ -7078,13 +7076,13 @@
         <v>197</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="I13" s="29" t="s">
+        <v>412</v>
+      </c>
+      <c r="I13" s="28" t="s">
         <v>3</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>198</v>
@@ -7092,8 +7090,8 @@
       <c r="L13" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="N13" s="29"/>
-      <c r="P13" s="29"/>
+      <c r="N13" s="28"/>
+      <c r="P13" s="28"/>
       <c r="Q13" s="6" t="s">
         <v>5</v>
       </c>
@@ -7121,7 +7119,7 @@
         <v>42</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>3</v>
@@ -7161,7 +7159,7 @@
         <v>282</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>3</v>
@@ -7170,7 +7168,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
@@ -7197,7 +7195,7 @@
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>3</v>
@@ -7223,7 +7221,7 @@
         <v>34</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>308</v>
@@ -7244,10 +7242,10 @@
         <v>3</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -7406,10 +7404,10 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="N35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P43" sqref="P43"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7505,20 +7503,20 @@
       <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>380</v>
+      <c r="H2" s="32" t="s">
+        <v>474</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>474</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>473</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>318</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>5</v>
@@ -7543,20 +7541,20 @@
       <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>380</v>
+      <c r="H3" s="32" t="s">
+        <v>474</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>474</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>473</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>318</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
@@ -7597,7 +7595,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>294</v>
@@ -7632,7 +7630,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -7652,7 +7650,7 @@
         <v>142</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>12</v>
@@ -7673,7 +7671,7 @@
         <v>112</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>9</v>
@@ -7766,19 +7764,19 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>411</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>413</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>414</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>174</v>
@@ -7845,7 +7843,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>9</v>
@@ -7853,10 +7851,10 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>174</v>
@@ -7871,7 +7869,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -7929,7 +7927,7 @@
         <v>4</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>5</v>
@@ -7996,7 +7994,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>9</v>
@@ -8004,7 +8002,7 @@
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>174</v>
@@ -8022,7 +8020,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -8054,7 +8052,7 @@
         <v>4</v>
       </c>
       <c r="P18" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>9</v>
@@ -8071,10 +8069,10 @@
         <v>11</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>174</v>
@@ -8092,7 +8090,7 @@
         <v>4</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>9</v>
@@ -8193,7 +8191,7 @@
         <v>95</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>256</v>
@@ -8214,7 +8212,7 @@
         <v>3</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>9</v>
@@ -8249,7 +8247,7 @@
         <v>4</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="Q24" s="6" t="s">
         <v>9</v>
@@ -8441,7 +8439,7 @@
         <v>4</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>9</v>
@@ -8470,7 +8468,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -8516,13 +8514,13 @@
     </row>
     <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>174</v>
@@ -8537,7 +8535,7 @@
         <v>4</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>9</v>
@@ -8601,7 +8599,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>9</v>
@@ -8697,7 +8695,7 @@
         <v>4</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>9</v>
@@ -8705,13 +8703,13 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>174</v>
@@ -8726,13 +8724,13 @@
         <v>4</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="Q39" s="6" t="s">
         <v>9</v>
@@ -8775,7 +8773,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>57</v>
@@ -8793,7 +8791,7 @@
         <v>4</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="Q41" s="6" t="s">
         <v>5</v>
@@ -8845,7 +8843,7 @@
         <v>338</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="Q43" s="6" t="s">
         <v>5</v>
@@ -9043,7 +9041,7 @@
         <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9051,7 +9049,7 @@
         <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -9075,7 +9073,7 @@
         <v>221</v>
       </c>
       <c r="B6" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9083,7 +9081,7 @@
         <v>227</v>
       </c>
       <c r="B7" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -9447,10 +9445,10 @@
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
@@ -9506,7 +9504,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>342</v>

</xml_diff>

<commit_message>
fixed bug with sex not selected correctly for CWD new countries and sampling areas
</commit_message>
<xml_diff>
--- a/compat/tablesSchema.2.0.0.xlsx
+++ b/compat/tablesSchema.2.0.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eclipse_workspace\tse_workspace\tse-reporting-tool\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F81ACC-F539-4C31-B5DC-38177CC851BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5A2279-15D2-4B51-BCB2-57EF97203EE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2916" yWindow="1440" windowWidth="20124" windowHeight="9720" tabRatio="690" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="690" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -1188,274 +1188,274 @@
     <t>sexLists</t>
   </si>
   <si>
+    <t>(RELATION{SummarizedInformation,type.code}==RGT)</t>
+  </si>
+  <si>
+    <t>%progLegalRef.code|IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},.|RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
+  </si>
+  <si>
+    <t>reportLastMessageId</t>
+  </si>
+  <si>
+    <t>reportLastModifyingMessageId</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH, used with Refresh Status/Display ack</t>
+  </si>
+  <si>
+    <t>A04MQ#RELATION{SummarizedInformation,source.code}$RELATION{CasesInformation,part.code}$RELATION{SummarizedInformation,prod.code}|IF_NOT_NULL(%animage.code,$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
+  </si>
+  <si>
+    <t>A04MQ#%source.code$%prod.code|IF((%type.code!=RGT),$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(%PSUId.label,PSUId=%PSUId.label,)</t>
+  </si>
+  <si>
+    <t>PSUId</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)|IF_NOT_NULL(RELATION{SummarizedInformation,PSUId.label},$PSUId=RELATION{SummarizedInformation,PSUId.label},)</t>
+  </si>
+  <si>
+    <t>Sample/case assessment</t>
+  </si>
+  <si>
+    <t>First test type</t>
+  </si>
+  <si>
+    <t>First test</t>
+  </si>
+  <si>
+    <t>Type of the first executed test</t>
+  </si>
+  <si>
+    <t>First executed test</t>
+  </si>
+  <si>
+    <t>sampInfo</t>
+  </si>
+  <si>
+    <t>D.11</t>
+  </si>
+  <si>
+    <t>origSampId</t>
+  </si>
+  <si>
+    <t>sampUnitType</t>
+  </si>
+  <si>
+    <t>C.02</t>
+  </si>
+  <si>
+    <t>G199A</t>
+  </si>
+  <si>
+    <t>H.01</t>
+  </si>
+  <si>
+    <t>anPortSeq</t>
+  </si>
+  <si>
+    <t>Portion</t>
+  </si>
+  <si>
+    <t>Portion of the analyzed sample</t>
+  </si>
+  <si>
+    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>sampEventAsses</t>
+  </si>
+  <si>
+    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,prod.code}==F21.A07RV),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,tseNationalCaseId.label},tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}$,)|IF_NOT_NULL(RELATION{CasesInformation,tseIndexCase.code},tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}$,)|IF_NOT_NULL(RELATION{CasesInformation,sampEventAsses.code},sampEventAsses=RELATION{CasesInformation,sampEventAsses.code},)|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
+  </si>
+  <si>
+    <t>cwdExtCont</t>
+  </si>
+  <si>
+    <t>pref11</t>
+  </si>
+  <si>
+    <t>yesNoLists</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Sex of the animals</t>
+  </si>
+  <si>
+    <t>%type.code|$%anMethType.code</t>
+  </si>
+  <si>
+    <t>(%type.code==SCRAPIE)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>OR((%type.code==CWD),(%type.code==BSEOS))</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,birthCountry.code},birthCountry=RELATION{CasesInformation,birthCountry.code},)|IF_NOT_NULL(RELATION{SummarizedInformation,statusHerd.code},$statusHerd=RELATION{SummarizedInformation,statusHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthInFlockHerd.code},$birthInFlockHerd=RELATION{CasesInformation,birthInFlockHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthYear.code},$birthYear=RELATION{CasesInformation,birthYear.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthMonth.code},$birthMonth=RELATION{CasesInformation,birthMonth.code},)</t>
+  </si>
+  <si>
+    <t>Herd/Flock status</t>
+  </si>
+  <si>
+    <t>Husbandry system</t>
+  </si>
+  <si>
+    <t>Aggregated-Data-(Level-1)</t>
+  </si>
+  <si>
+    <t>Sample-Level-Data-(Level-2)</t>
+  </si>
+  <si>
+    <t>Analytical-Test-Results-(Level-3)</t>
+  </si>
+  <si>
+    <t>Report-Management</t>
+  </si>
+  <si>
+    <t>%progId.label|.0</t>
+  </si>
+  <si>
+    <t>%progId.label</t>
+  </si>
+  <si>
+    <t>NEXT(,)</t>
+  </si>
+  <si>
+    <t>Dataset ID</t>
+  </si>
+  <si>
+    <t>Report Status</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT), origSampId=%sampId.label, )</t>
+  </si>
+  <si>
+    <t>(%type.code==RGT)</t>
+  </si>
+  <si>
+    <t>F01.A057G</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),RF-00004629-PAR#allele=%allele1.label$allele=%allele2.label,RF-00004628-PAR)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),0,)</t>
+  </si>
+  <si>
+    <t>IF(OR((%type.code!=CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F32.A0C9B,)</t>
+  </si>
+  <si>
+    <t>(RELATION{SummarizedInformation,sex.code}==F32.A0C9B)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,sex.code}!=F32.A0C9B),RELATION{SummarizedInformation,sex.code},)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F01.A056M,)</t>
+  </si>
+  <si>
+    <t>AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==Y))</t>
+  </si>
+  <si>
+    <t>(%type.code==CWD)</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT),tseTargetGroup=%tseTargetGroup.code$totSamplesTested=%totSamplesTested.label$totSamplesPositive=%totSamplesPositive.label$totSamplesNegative=%totSamplesNegative.label$totSamplesInconclusive=%totSamplesInconclusive.label$totSamplesUnsuitable=%totSamplesUnsuitable.label,totSamplesTested=%totSamplesTested.label)</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT),SUM(%totSamplesPositive.label,%totSamplesNegative.label,%totSamplesInconclusive.label),)</t>
+  </si>
+  <si>
+    <t>PSU id required</t>
+  </si>
+  <si>
+    <t>Flag to include Primary Sample Unit as mandatory field</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)</t>
+  </si>
+  <si>
+    <t>(%sampEventAsses.code!=J051A)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),AT13A,AT06A)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)IF((%type.code==RGT),F089A,)</t>
+  </si>
+  <si>
+    <t>SCRAPIE$AT06A</t>
+  </si>
+  <si>
+    <t>IF((%type.code==SCRAPIE),BSE,%type.code)</t>
+  </si>
+  <si>
+    <t>origSampId=%origSampId.label</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,animage.code}</t>
+  </si>
+  <si>
+    <t>%paramCodeBaseTerm.code</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,progId.label}|.%progIdSuffix.code</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,type.code}$%anMethType.code</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,sampId.label}</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,type.code}%anMethType.code</t>
+  </si>
+  <si>
+    <t>IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),F,)</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>RELATION{Preferences,country.code}|RIGHT_TRIM(lastMonth.year.code,2)|RIGHT_TRIM(ZERO_PADDING(lastMonth.code,2),2)</t>
+  </si>
+  <si>
+    <t>%country.code|RIGHT_TRIM(%reportYear.code,2)|RIGHT_TRIM(ZERO_PADDING(%reportMonth.code,2),2)</t>
+  </si>
+  <si>
+    <t>CWD$AT11A</t>
+  </si>
+  <si>
+    <t>2021 to 2050</t>
+  </si>
+  <si>
+    <t>OR((RELATION{SummarizedInformation,source.code}==F01.A057G),(RELATION{SummarizedInformation,source.code}==F01.A057P))</t>
+  </si>
+  <si>
+    <t>IF((%anMethType.code==AT13A),OR((RELATION{SummarizedInformation,source.code}==F01.A057G),(RELATION{SummarizedInformation,source.code}==F01.A057P)),No)</t>
+  </si>
+  <si>
+    <t>RELATION{CasesInformation,sex.code}</t>
+  </si>
+  <si>
     <t>FM</t>
-  </si>
-  <si>
-    <t>(RELATION{SummarizedInformation,type.code}==RGT)</t>
-  </si>
-  <si>
-    <t>%progLegalRef.code|IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},.|RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
-  </si>
-  <si>
-    <t>reportLastMessageId</t>
-  </si>
-  <si>
-    <t>reportLastModifyingMessageId</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH, used with Refresh Status/Display ack</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}==CWD),RELATION{SummarizedInformation,sex.code},RELATION{CasesInformation,sex.code})</t>
-  </si>
-  <si>
-    <t>A04MQ#RELATION{SummarizedInformation,source.code}$RELATION{CasesInformation,part.code}$RELATION{SummarizedInformation,prod.code}|IF_NOT_NULL(%animage.code,$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
-  </si>
-  <si>
-    <t>A04MQ#%source.code$%prod.code|IF((%type.code!=RGT),$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(%PSUId.label,PSUId=%PSUId.label,)</t>
-  </si>
-  <si>
-    <t>PSUId</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)|IF_NOT_NULL(RELATION{SummarizedInformation,PSUId.label},$PSUId=RELATION{SummarizedInformation,PSUId.label},)</t>
-  </si>
-  <si>
-    <t>Sample/case assessment</t>
-  </si>
-  <si>
-    <t>First test type</t>
-  </si>
-  <si>
-    <t>First test</t>
-  </si>
-  <si>
-    <t>Type of the first executed test</t>
-  </si>
-  <si>
-    <t>First executed test</t>
-  </si>
-  <si>
-    <t>sampInfo</t>
-  </si>
-  <si>
-    <t>D.11</t>
-  </si>
-  <si>
-    <t>origSampId</t>
-  </si>
-  <si>
-    <t>sampUnitType</t>
-  </si>
-  <si>
-    <t>C.02</t>
-  </si>
-  <si>
-    <t>G199A</t>
-  </si>
-  <si>
-    <t>H.01</t>
-  </si>
-  <si>
-    <t>anPortSeq</t>
-  </si>
-  <si>
-    <t>Portion</t>
-  </si>
-  <si>
-    <t>Portion of the analyzed sample</t>
-  </si>
-  <si>
-    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
-    <t>sampEventAsses</t>
-  </si>
-  <si>
-    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,prod.code}==F21.A07RV),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,tseNationalCaseId.label},tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}$,)|IF_NOT_NULL(RELATION{CasesInformation,tseIndexCase.code},tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}$,)|IF_NOT_NULL(RELATION{CasesInformation,sampEventAsses.code},sampEventAsses=RELATION{CasesInformation,sampEventAsses.code},)|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
-  </si>
-  <si>
-    <t>cwdExtCont</t>
-  </si>
-  <si>
-    <t>pref11</t>
-  </si>
-  <si>
-    <t>yesNoLists</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Sex of the animals</t>
-  </si>
-  <si>
-    <t>%type.code|$%anMethType.code</t>
-  </si>
-  <si>
-    <t>(%type.code==SCRAPIE)</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>OR((%type.code==CWD),(%type.code==BSEOS))</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,birthCountry.code},birthCountry=RELATION{CasesInformation,birthCountry.code},)|IF_NOT_NULL(RELATION{SummarizedInformation,statusHerd.code},$statusHerd=RELATION{SummarizedInformation,statusHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthInFlockHerd.code},$birthInFlockHerd=RELATION{CasesInformation,birthInFlockHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthYear.code},$birthYear=RELATION{CasesInformation,birthYear.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthMonth.code},$birthMonth=RELATION{CasesInformation,birthMonth.code},)</t>
-  </si>
-  <si>
-    <t>Herd/Flock status</t>
-  </si>
-  <si>
-    <t>Husbandry system</t>
-  </si>
-  <si>
-    <t>Aggregated-Data-(Level-1)</t>
-  </si>
-  <si>
-    <t>Sample-Level-Data-(Level-2)</t>
-  </si>
-  <si>
-    <t>Analytical-Test-Results-(Level-3)</t>
-  </si>
-  <si>
-    <t>Report-Management</t>
-  </si>
-  <si>
-    <t>%progId.label|.0</t>
-  </si>
-  <si>
-    <t>%progId.label</t>
-  </si>
-  <si>
-    <t>NEXT(,)</t>
-  </si>
-  <si>
-    <t>Dataset ID</t>
-  </si>
-  <si>
-    <t>Report Status</t>
-  </si>
-  <si>
-    <t>IF((%type.code!=RGT), origSampId=%sampId.label, )</t>
-  </si>
-  <si>
-    <t>(%type.code==RGT)</t>
-  </si>
-  <si>
-    <t>F01.A057G</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),RF-00004629-PAR#allele=%allele1.label$allele=%allele2.label,RF-00004628-PAR)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),0,)</t>
-  </si>
-  <si>
-    <t>IF(OR((%type.code!=CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F32.A0C9B,)</t>
-  </si>
-  <si>
-    <t>(RELATION{SummarizedInformation,sex.code}==F32.A0C9B)</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,sex.code}!=F32.A0C9B),RELATION{SummarizedInformation,sex.code},)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F01.A056M,)</t>
-  </si>
-  <si>
-    <t>AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==Y))</t>
-  </si>
-  <si>
-    <t>(%type.code==CWD)</t>
-  </si>
-  <si>
-    <t>IF((%type.code!=RGT),tseTargetGroup=%tseTargetGroup.code$totSamplesTested=%totSamplesTested.label$totSamplesPositive=%totSamplesPositive.label$totSamplesNegative=%totSamplesNegative.label$totSamplesInconclusive=%totSamplesInconclusive.label$totSamplesUnsuitable=%totSamplesUnsuitable.label,totSamplesTested=%totSamplesTested.label)</t>
-  </si>
-  <si>
-    <t>IF((%type.code!=RGT),SUM(%totSamplesPositive.label,%totSamplesNegative.label,%totSamplesInconclusive.label),)</t>
-  </si>
-  <si>
-    <t>PSU id required</t>
-  </si>
-  <si>
-    <t>Flag to include Primary Sample Unit as mandatory field</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)</t>
-  </si>
-  <si>
-    <t>(%sampEventAsses.code!=J051A)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),AT13A,AT06A)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)IF((%type.code==RGT),F089A,)</t>
-  </si>
-  <si>
-    <t>SCRAPIE$AT06A</t>
-  </si>
-  <si>
-    <t>IF((%type.code==SCRAPIE),BSE,%type.code)</t>
-  </si>
-  <si>
-    <t>origSampId=%origSampId.label</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,animage.code}</t>
-  </si>
-  <si>
-    <t>%paramCodeBaseTerm.code</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,progId.label}|.%progIdSuffix.code</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,type.code}$%anMethType.code</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,sampId.label}</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,type.code}%anMethType.code</t>
-  </si>
-  <si>
-    <t>IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),F,)</t>
-  </si>
-  <si>
-    <t>POS</t>
-  </si>
-  <si>
-    <t>RELATION{Preferences,country.code}|RIGHT_TRIM(lastMonth.year.code,2)|RIGHT_TRIM(ZERO_PADDING(lastMonth.code,2),2)</t>
-  </si>
-  <si>
-    <t>%country.code|RIGHT_TRIM(%reportYear.code,2)|RIGHT_TRIM(ZERO_PADDING(%reportMonth.code,2),2)</t>
-  </si>
-  <si>
-    <t>CWD$AT11A</t>
-  </si>
-  <si>
-    <t>2021 to 2050</t>
-  </si>
-  <si>
-    <t>OR((RELATION{SummarizedInformation,source.code}==F01.A057G),(RELATION{SummarizedInformation,source.code}==F01.A057P))</t>
-  </si>
-  <si>
-    <t>IF((%anMethType.code==AT13A),OR((RELATION{SummarizedInformation,source.code}==F01.A057G),(RELATION{SummarizedInformation,source.code}==F01.A057P)),No)</t>
   </si>
 </sst>
 </file>
@@ -3953,16 +3953,16 @@
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F3" s="24" t="s">
         <v>12</v>
@@ -3980,16 +3980,16 @@
         <v>9</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>9</v>
@@ -4071,7 +4071,7 @@
         <v>112</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R5" s="2">
         <v>4</v>
@@ -4340,7 +4340,7 @@
         <v>112</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
@@ -4469,7 +4469,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>9</v>
@@ -4583,10 +4583,10 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4712,7 +4712,7 @@
       <c r="C8" s="17"/>
       <c r="D8" s="18"/>
       <c r="E8" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>174</v>
@@ -4743,13 +4743,13 @@
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="18"/>
       <c r="E9" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>174</v>
@@ -4780,13 +4780,13 @@
     </row>
     <row r="10" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
       <c r="E10" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>174</v>
@@ -4824,10 +4824,10 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>174</v>
@@ -4867,10 +4867,10 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>174</v>
@@ -4954,10 +4954,10 @@
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P23" sqref="P23"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5118,10 +5118,10 @@
         <v>311</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
@@ -5141,7 +5141,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>69</v>
@@ -5156,7 +5156,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>3</v>
@@ -5276,10 +5276,10 @@
         <v>57</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>12</v>
@@ -5291,7 +5291,7 @@
         <v>3</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>3</v>
@@ -5303,7 +5303,7 @@
         <v>311</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="6" t="s">
@@ -5327,10 +5327,10 @@
         <v>89</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>398</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>400</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>12</v>
@@ -5351,13 +5351,13 @@
         <v>307</v>
       </c>
       <c r="L8" s="28" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>9</v>
@@ -5380,10 +5380,10 @@
         <v>92</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>399</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>401</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>12</v>
@@ -5404,13 +5404,13 @@
         <v>112</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="Q9" s="6" t="s">
         <v>9</v>
@@ -5430,7 +5430,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>36</v>
@@ -5442,10 +5442,10 @@
         <v>37</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>3</v>
@@ -5457,10 +5457,10 @@
         <v>311</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="Q10" s="6" t="s">
         <v>5</v>
@@ -5474,23 +5474,23 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>202</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>174</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>3</v>
@@ -5639,19 +5639,19 @@
         <v>8</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
@@ -5727,7 +5727,7 @@
         <v>3</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>9</v>
@@ -5754,10 +5754,10 @@
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>3</v>
@@ -5766,7 +5766,7 @@
         <v>318</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>5</v>
@@ -5796,10 +5796,10 @@
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>3</v>
@@ -5808,7 +5808,7 @@
         <v>318</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>5</v>
@@ -5936,7 +5936,7 @@
         <v>4</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>9</v>
@@ -6023,7 +6023,7 @@
         <v>4</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="Q26" s="6" t="s">
         <v>9</v>
@@ -6174,7 +6174,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -6206,7 +6206,7 @@
         <v>4</v>
       </c>
       <c r="P32" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>9</v>
@@ -6270,7 +6270,7 @@
         <v>4</v>
       </c>
       <c r="P34" s="6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="Q34" s="6" t="s">
         <v>9</v>
@@ -6302,7 +6302,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>9</v>
@@ -6310,13 +6310,13 @@
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>174</v>
@@ -6331,7 +6331,7 @@
         <v>4</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="Q36" s="6" t="s">
         <v>9</v>
@@ -6398,7 +6398,7 @@
         <v>4</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>9</v>
@@ -6459,7 +6459,7 @@
         <v>4</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="Q40" s="6" t="s">
         <v>9</v>
@@ -6534,10 +6534,10 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD13"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6624,13 +6624,13 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B2" t="s">
         <v>191</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>211</v>
@@ -6756,10 +6756,10 @@
         <v>57</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>12</v>
@@ -6768,10 +6768,10 @@
         <v>381</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>3</v>
@@ -6780,10 +6780,10 @@
         <v>384</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>385</v>
+        <v>474</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -6812,10 +6812,10 @@
         <v>74</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>4</v>
@@ -6853,7 +6853,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>3</v>
@@ -6891,7 +6891,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>3</v>
@@ -7035,7 +7035,7 @@
         <v>217</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>3</v>
@@ -7076,7 +7076,7 @@
         <v>197</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I13" s="28" t="s">
         <v>3</v>
@@ -7119,7 +7119,7 @@
         <v>42</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>3</v>
@@ -7159,7 +7159,7 @@
         <v>282</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>3</v>
@@ -7195,7 +7195,7 @@
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>3</v>
@@ -7242,10 +7242,10 @@
         <v>3</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -7404,10 +7404,10 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7504,13 +7504,13 @@
         <v>12</v>
       </c>
       <c r="H2" s="32" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>318</v>
@@ -7542,13 +7542,13 @@
         <v>12</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="J3" s="32" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>318</v>
@@ -7630,7 +7630,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -7671,7 +7671,7 @@
         <v>112</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>9</v>
@@ -7764,19 +7764,19 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>408</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>409</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>410</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>411</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>174</v>
@@ -7843,7 +7843,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>9</v>
@@ -7851,10 +7851,10 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>174</v>
@@ -7869,7 +7869,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -7927,7 +7927,7 @@
         <v>4</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>5</v>
@@ -7994,7 +7994,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>9</v>
@@ -8020,7 +8020,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -8247,7 +8247,7 @@
         <v>4</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="Q24" s="6" t="s">
         <v>9</v>
@@ -8468,7 +8468,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -8514,13 +8514,13 @@
     </row>
     <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>174</v>
@@ -8535,7 +8535,7 @@
         <v>4</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>9</v>
@@ -8599,7 +8599,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>9</v>
@@ -8695,7 +8695,7 @@
         <v>4</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>9</v>
@@ -8703,13 +8703,13 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>174</v>
@@ -8724,13 +8724,13 @@
         <v>4</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="Q39" s="6" t="s">
         <v>9</v>
@@ -8790,8 +8790,8 @@
       <c r="J41" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N41" s="6" t="s">
-        <v>391</v>
+      <c r="N41" s="32" t="s">
+        <v>473</v>
       </c>
       <c r="Q41" s="6" t="s">
         <v>5</v>
@@ -8843,7 +8843,7 @@
         <v>338</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="Q43" s="6" t="s">
         <v>5</v>
@@ -9041,7 +9041,7 @@
         <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9049,7 +9049,7 @@
         <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -9073,7 +9073,7 @@
         <v>221</v>
       </c>
       <c r="B6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9081,7 +9081,7 @@
         <v>227</v>
       </c>
       <c r="B7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -9100,7 +9100,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>